<commit_message>
Correções apresentadas pelo sonar
</commit_message>
<xml_diff>
--- a/src/test/resources/br/gov/sp/fatec/mapskills/file/import-institutions.xlsx
+++ b/src/test/resources/br/gov/sp/fatec/mapskills/file/import-institutions.xlsx
@@ -1,10 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="19029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcelo\Documents\GitHub\mapskills-engine\src\test\resources\br\gov\sp\fatec\mapskills\file\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{05D230E7-3BC7-4CE8-80BE-718173432DAA}" xr6:coauthVersionLast="28" xr6:coauthVersionMax="28" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -54,9 +60,6 @@
     <t>São Paulo</t>
   </si>
   <si>
-    <t>Pref. Hirant Sanazar</t>
-  </si>
-  <si>
     <t>Osasco</t>
   </si>
   <si>
@@ -84,9 +87,6 @@
     <t>Técnico</t>
   </si>
   <si>
-    <t>Profª Ilza Nascimento Pintus</t>
-  </si>
-  <si>
     <t>benício.barros@etec.sp.gov.br</t>
   </si>
   <si>
@@ -94,13 +94,19 @@
   </si>
   <si>
     <t>thomas.santos@etec.sp.gov.br</t>
+  </si>
+  <si>
+    <t>Prof. Hirant Sanazar</t>
+  </si>
+  <si>
+    <t>Prof. Ilza Nascimento Pintus</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -110,6 +116,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -135,11 +149,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="12" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -150,6 +165,9 @@
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
     </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
   </extLst>
 </styleSheet>
 </file>
@@ -157,7 +175,7 @@
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema do Office">
   <a:themeElements>
-    <a:clrScheme name="Escritório">
+    <a:clrScheme name="Office">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -195,9 +213,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Escritório">
+    <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -230,9 +248,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -265,9 +300,26 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Escritório">
+    <a:fmtScheme name="Office">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -440,11 +492,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -498,10 +550,10 @@
         <v>9</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -521,10 +573,10 @@
         <v>11</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="G3" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -535,19 +587,19 @@
         <v>46532670000150</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="F4" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>18</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>19</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -558,33 +610,34 @@
         <v>60422037000130</v>
       </c>
       <c r="C5" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="D5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E5" s="1" t="s">
         <v>9</v>
       </c>
       <c r="F5" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
-        <v>24</v>
-      </c>
+        <v>22</v>
+      </c>
+      <c r="C6" s="4"/>
       <c r="D6" s="1" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="E6" s="1" t="s">
         <v>9</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -594,7 +647,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
@@ -606,7 +659,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>

</xml_diff>